<commit_message>
fix memory leak. fix lua function bugs.
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -1,15 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -19,19 +18,30 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>中文测试</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -41,13 +51,47 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -59,14 +103,57 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="常规 2" xfId="2"/>
+    <cellStyle name="常规 2 2" xfId="5"/>
+    <cellStyle name="常规 3" xfId="1"/>
+    <cellStyle name="常规 3 2" xfId="4"/>
+    <cellStyle name="常规 4" xfId="6"/>
+    <cellStyle name="常规 4 2" xfId="7"/>
+    <cellStyle name="常规 5" xfId="3"/>
+    <cellStyle name="常规 6" xfId="10"/>
+    <cellStyle name="好 2" xfId="9"/>
+    <cellStyle name="好 3" xfId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -365,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -445,8 +532,19 @@
         <v>8</v>
       </c>
     </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="B14" s="2">
+        <v>42437</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -456,24 +554,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="2" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>